<commit_message>
removal of IMAIZUMI, fuck that guy and his smart Tokio equations
</commit_message>
<xml_diff>
--- a/bin/Debug/Log.xlsx
+++ b/bin/Debug/Log.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="142">
   <si>
     <t>Simulation</t>
   </si>
@@ -1184,11 +1184,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="458891288"/>
-        <c:axId val="458893640"/>
+        <c:axId val="238805512"/>
+        <c:axId val="238804728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="458891288"/>
+        <c:axId val="238805512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458893640"/>
+        <c:crossAx val="238804728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1301,7 +1301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="458893640"/>
+        <c:axId val="238804728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458891288"/>
+        <c:crossAx val="238805512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2007,11 +2007,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="316962024"/>
-        <c:axId val="316961240"/>
+        <c:axId val="238800808"/>
+        <c:axId val="238800416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316962024"/>
+        <c:axId val="238800808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,7 +2085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316961240"/>
+        <c:crossAx val="238800416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2093,7 +2093,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316961240"/>
+        <c:axId val="238800416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316962024"/>
+        <c:crossAx val="238800808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2685,11 +2685,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="309417744"/>
-        <c:axId val="309416568"/>
+        <c:axId val="238800024"/>
+        <c:axId val="238797672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="309417744"/>
+        <c:axId val="238800024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,7 +2732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309416568"/>
+        <c:crossAx val="238797672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2740,7 +2740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309416568"/>
+        <c:axId val="238797672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2764,7 +2764,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309417744"/>
+        <c:crossAx val="238800024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4454,8 +4454,8 @@
     <xdr:to>
       <xdr:col>55</xdr:col>
       <xdr:colOff>388793</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>225136</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4477,15 +4477,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>34637</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>472784</xdr:rowOff>
+      <xdr:colOff>79460</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>187034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>484909</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>173181</xdr:rowOff>
+      <xdr:colOff>529732</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4506,16 +4506,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161058</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>39220</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>149852</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>536863</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>480835</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>144658</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4810,17 +4810,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="F14" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="3" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="2" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15" style="7" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="20.140625" style="5" customWidth="1"/>
@@ -7441,7 +7441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>0</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>0</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>0</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>0</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>0</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>0</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>0</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>0</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>0</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>0</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>0</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>0</v>
       </c>
@@ -7857,7 +7857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>0</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>0</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>0</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>0</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>0</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>0</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>0</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>0</v>
       </c>
@@ -8151,7 +8151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>0</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -8221,7 +8221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>0</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>0</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>0</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>0</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>0</v>
       </c>
@@ -8396,7 +8396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>0</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>0</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>0</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>0</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>0</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>0</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>0</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>0</v>
       </c>
@@ -8655,7 +8655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>0</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>0</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>0</v>
       </c>
@@ -10071,8 +10071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AY64" sqref="AY64"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ31" sqref="AJ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10090,7 +10090,8 @@
     <col min="12" max="32" width="9.140625" style="2"/>
     <col min="33" max="33" width="12" style="7" customWidth="1"/>
     <col min="34" max="34" width="21.85546875" style="9" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="2"/>
+    <col min="35" max="35" width="13.5703125" style="2" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -10103,9 +10104,7 @@
       <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
@@ -10115,16 +10114,10 @@
       <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="2" t="s">
         <v>21</v>
@@ -10145,7 +10138,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>('Full data'!A2)</f>
         <v>Simulation</v>
@@ -10158,10 +10151,6 @@
         <f>('Full data'!C2)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="str">
-        <f>('Full data'!D2)</f>
-        <v>2015-05-15.10:38:00</v>
-      </c>
       <c r="E2" s="10" t="s">
         <v>136</v>
       </c>
@@ -10173,22 +10162,10 @@
         <f>('Full data'!G2)</f>
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="str">
-        <f>('Full data'!H2)</f>
-        <v xml:space="preserve">Row: 1 Column: 1 Row: 3 Column: 3 Row: 5 Column: 5 </v>
-      </c>
       <c r="I2" s="2" t="str">
         <f>('Full data'!I2)</f>
         <v>B</v>
       </c>
-      <c r="J2" s="2" t="str">
-        <f>('Full data'!J2)</f>
-        <v>[10,10](1,1)(8,8))</v>
-      </c>
-      <c r="K2" s="2" t="str">
-        <f>('Full data'!K2)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AE2" s="2" t="s">
         <v>11</v>
       </c>
@@ -10209,7 +10186,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>('Full data'!A12)</f>
         <v>Simulation</v>
@@ -10222,10 +10199,6 @@
         <f>('Full data'!C12)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="str">
-        <f>('Full data'!D12)</f>
-        <v>2015-05-15.10:38:05</v>
-      </c>
       <c r="E3" s="10" t="s">
         <v>137</v>
       </c>
@@ -10237,22 +10210,10 @@
         <f>('Full data'!G12)</f>
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="str">
-        <f>('Full data'!H12)</f>
-        <v xml:space="preserve">Row: 4 Column: 4 Row: 7 Column: 7 </v>
-      </c>
       <c r="I3" s="2" t="str">
         <f>('Full data'!I12)</f>
         <v>B</v>
       </c>
-      <c r="J3" s="2" t="str">
-        <f>('Full data'!J12)</f>
-        <v>[10,10](1,1)(8,8))</v>
-      </c>
-      <c r="K3" s="2" t="str">
-        <f>('Full data'!K12)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF3" s="2" t="s">
         <v>137</v>
       </c>
@@ -10270,7 +10231,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>('Full data'!A22)</f>
         <v>Simulation</v>
@@ -10283,10 +10244,6 @@
         <f>('Full data'!C22)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>('Full data'!D22)</f>
-        <v>2015-05-15.10:38:08</v>
-      </c>
       <c r="E4" s="10" t="s">
         <v>138</v>
       </c>
@@ -10298,22 +10255,10 @@
         <f>('Full data'!G22)</f>
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="str">
-        <f>('Full data'!H22)</f>
-        <v xml:space="preserve">Row: 2 Column: 2 Row: 4 Column: 4 Row: 6 Column: 6 </v>
-      </c>
       <c r="I4" s="2" t="str">
         <f>('Full data'!I22)</f>
         <v>B</v>
       </c>
-      <c r="J4" s="2" t="str">
-        <f>('Full data'!J22)</f>
-        <v>[10,10](1,1)(8,8))</v>
-      </c>
-      <c r="K4" s="2" t="str">
-        <f>('Full data'!K22)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF4" s="2" t="s">
         <v>138</v>
       </c>
@@ -10331,7 +10276,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>('Full data'!A32)</f>
         <v>Simulation</v>
@@ -10344,10 +10289,6 @@
         <f>('Full data'!C32)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <f>('Full data'!D32)</f>
-        <v>2015-05-15.10:38:11</v>
-      </c>
       <c r="E5" s="10" t="s">
         <v>139</v>
       </c>
@@ -10359,22 +10300,10 @@
         <f>('Full data'!G32)</f>
         <v>12</v>
       </c>
-      <c r="H5" s="2" t="str">
-        <f>('Full data'!H32)</f>
-        <v xml:space="preserve">Row: 2 Column: 2 Row: 4 Column: 4 Row: 6 Column: 6 </v>
-      </c>
       <c r="I5" s="2" t="str">
         <f>('Full data'!I32)</f>
         <v>B</v>
       </c>
-      <c r="J5" s="2" t="str">
-        <f>('Full data'!J32)</f>
-        <v>[10,10](1,1)(8,8))</v>
-      </c>
-      <c r="K5" s="2" t="str">
-        <f>('Full data'!K32)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF5" s="2" t="s">
         <v>139</v>
       </c>
@@ -10392,7 +10321,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>('Full data'!A42)</f>
         <v>Simulation</v>
@@ -10405,10 +10334,6 @@
         <f>('Full data'!C42)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f>('Full data'!D42)</f>
-        <v>2015-05-15.10:38:13</v>
-      </c>
       <c r="E6" s="10" t="s">
         <v>136</v>
       </c>
@@ -10420,22 +10345,10 @@
         <f>('Full data'!G42)</f>
         <v>6</v>
       </c>
-      <c r="H6" s="2" t="str">
-        <f>('Full data'!H42)</f>
-        <v xml:space="preserve">Row: 3 Column: 3 Row: 5 Column: 5 Row: 7 Column: 7 </v>
-      </c>
       <c r="I6" s="2" t="str">
         <f>('Full data'!I42)</f>
         <v>C</v>
       </c>
-      <c r="J6" s="2" t="str">
-        <f>('Full data'!J42)</f>
-        <v>[10,10](8,8)(1,1))</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f>('Full data'!K42)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AE6" s="2" t="s">
         <v>12</v>
       </c>
@@ -10456,7 +10369,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>('Full data'!A52)</f>
         <v>Simulation</v>
@@ -10469,10 +10382,6 @@
         <f>('Full data'!C52)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f>('Full data'!D52)</f>
-        <v>2015-05-15.10:38:18</v>
-      </c>
       <c r="E7" s="10" t="s">
         <v>137</v>
       </c>
@@ -10484,22 +10393,10 @@
         <f>('Full data'!G52)</f>
         <v>6</v>
       </c>
-      <c r="H7" s="2" t="str">
-        <f>('Full data'!H52)</f>
-        <v xml:space="preserve">Row: 1 Column: 1 Row: 4 Column: 4 </v>
-      </c>
       <c r="I7" s="2" t="str">
         <f>('Full data'!I52)</f>
         <v>C</v>
       </c>
-      <c r="J7" s="2" t="str">
-        <f>('Full data'!J52)</f>
-        <v>[10,10](8,8)(1,1))</v>
-      </c>
-      <c r="K7" s="2" t="str">
-        <f>('Full data'!K52)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF7" s="2" t="s">
         <v>137</v>
       </c>
@@ -10517,7 +10414,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>('Full data'!A62)</f>
         <v>Simulation</v>
@@ -10530,10 +10427,6 @@
         <f>('Full data'!C62)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="str">
-        <f>('Full data'!D62)</f>
-        <v>2015-05-15.10:38:21</v>
-      </c>
       <c r="E8" s="10" t="s">
         <v>138</v>
       </c>
@@ -10545,22 +10438,10 @@
         <f>('Full data'!G62)</f>
         <v>10</v>
       </c>
-      <c r="H8" s="2" t="str">
-        <f>('Full data'!H62)</f>
-        <v xml:space="preserve">Row: 1 Column: 1 Row: 3 Column: 3 Row: 5 Column: 5 </v>
-      </c>
       <c r="I8" s="2" t="str">
         <f>('Full data'!I62)</f>
         <v>C</v>
       </c>
-      <c r="J8" s="2" t="str">
-        <f>('Full data'!J62)</f>
-        <v>[10,10](8,8)(1,1))</v>
-      </c>
-      <c r="K8" s="2" t="str">
-        <f>('Full data'!K62)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF8" s="2" t="s">
         <v>138</v>
       </c>
@@ -10578,7 +10459,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f>('Full data'!A72)</f>
         <v>Simulation</v>
@@ -10591,10 +10472,6 @@
         <f>('Full data'!C72)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f>('Full data'!D72)</f>
-        <v>2015-05-15.10:38:24</v>
-      </c>
       <c r="E9" s="10" t="s">
         <v>139</v>
       </c>
@@ -10606,22 +10483,10 @@
         <f>('Full data'!G72)</f>
         <v>10</v>
       </c>
-      <c r="H9" s="2" t="str">
-        <f>('Full data'!H72)</f>
-        <v xml:space="preserve">Row: 1 Column: 1 Row: 3 Column: 3 Row: 5 Column: 5 </v>
-      </c>
       <c r="I9" s="2" t="str">
         <f>('Full data'!I72)</f>
         <v>C</v>
       </c>
-      <c r="J9" s="2" t="str">
-        <f>('Full data'!J72)</f>
-        <v>[10,10](8,8)(1,1))</v>
-      </c>
-      <c r="K9" s="2" t="str">
-        <f>('Full data'!K72)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF9" s="2" t="s">
         <v>139</v>
       </c>
@@ -10639,7 +10504,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f>('Full data'!A82)</f>
         <v>Simulation</v>
@@ -10652,10 +10517,6 @@
         <f>('Full data'!C82)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>('Full data'!D82)</f>
-        <v>2015-05-15.10:38:27</v>
-      </c>
       <c r="E10" s="10" t="s">
         <v>136</v>
       </c>
@@ -10667,22 +10528,10 @@
         <f>('Full data'!G82)</f>
         <v>21</v>
       </c>
-      <c r="H10" s="2" t="str">
-        <f>('Full data'!H82)</f>
-        <v xml:space="preserve">Row: 2 Column: 9 Row: 2 Column: 11 Row: 4 Column: 11 </v>
-      </c>
       <c r="I10" s="2" t="str">
         <f>('Full data'!I82)</f>
         <v>D</v>
       </c>
-      <c r="J10" s="2" t="str">
-        <f>('Full data'!J82)</f>
-        <v>[10,20](1,1)(8,1)(4,0,1,10))</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <f>('Full data'!K82)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AE10" s="2" t="s">
         <v>13</v>
       </c>
@@ -10703,7 +10552,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f>('Full data'!A92)</f>
         <v>Simulation</v>
@@ -10716,10 +10565,6 @@
         <f>('Full data'!C92)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f>('Full data'!D92)</f>
-        <v>2015-05-15.10:38:37</v>
-      </c>
       <c r="E11" s="10" t="s">
         <v>137</v>
       </c>
@@ -10731,22 +10576,10 @@
         <f>('Full data'!G92)</f>
         <v>21</v>
       </c>
-      <c r="H11" s="2" t="str">
-        <f>('Full data'!H92)</f>
-        <v xml:space="preserve">Row: 2 Column: 9 Row: 2 Column: 11 Row: 4 Column: 11 </v>
-      </c>
       <c r="I11" s="2" t="str">
         <f>('Full data'!I92)</f>
         <v>D</v>
       </c>
-      <c r="J11" s="2" t="str">
-        <f>('Full data'!J92)</f>
-        <v>[10,20](1,1)(8,1)(4,0,1,10))</v>
-      </c>
-      <c r="K11" s="2" t="str">
-        <f>('Full data'!K92)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF11" s="2" t="s">
         <v>137</v>
       </c>
@@ -10764,7 +10597,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f>('Full data'!A102)</f>
         <v>Simulation</v>
@@ -10777,37 +10610,21 @@
         <f>('Full data'!C102)</f>
         <v>unreachable location presented</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>('Full data'!D102)</f>
-        <v>2015-05-15.10:38:46</v>
-      </c>
       <c r="E12" s="10" t="s">
         <v>138</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="2" t="str">
-        <f>('Full data'!H102)</f>
-        <v xml:space="preserve">Row: 1 Column: 20 Row: 1 Column: 21 </v>
-      </c>
       <c r="I12" s="2" t="str">
         <f>('Full data'!I102)</f>
         <v>D</v>
       </c>
-      <c r="J12" s="2" t="str">
-        <f>('Full data'!J102)</f>
-        <v>[10,20](1,1)(8,1)(4,0,1,10))</v>
-      </c>
-      <c r="K12" s="2" t="str">
-        <f>('Full data'!K102)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF12" s="2" t="s">
         <v>138</v>
       </c>
       <c r="AG12" s="5"/>
       <c r="AI12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f>('Full data'!A112)</f>
         <v>Simulation</v>
@@ -10820,10 +10637,6 @@
         <f>('Full data'!C112)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f>('Full data'!D112)</f>
-        <v>2015-05-15.10:38:51</v>
-      </c>
       <c r="E13" s="10" t="s">
         <v>139</v>
       </c>
@@ -10835,22 +10648,10 @@
         <f>('Full data'!G112)</f>
         <v>37</v>
       </c>
-      <c r="H13" s="2" t="str">
-        <f>('Full data'!H112)</f>
-        <v xml:space="preserve">Row: 2 Column: 10 Row: 2 Column: 11 Row: 2 Column: 15 </v>
-      </c>
       <c r="I13" s="2" t="str">
         <f>('Full data'!I112)</f>
         <v>D</v>
       </c>
-      <c r="J13" s="2" t="str">
-        <f>('Full data'!J112)</f>
-        <v>[10,20](1,1)(8,1)(4,0,1,10))</v>
-      </c>
-      <c r="K13" s="2" t="str">
-        <f>('Full data'!K112)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF13" s="2" t="s">
         <v>139</v>
       </c>
@@ -10868,7 +10669,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>('Full data'!A122)</f>
         <v>Simulation</v>
@@ -10881,30 +10682,14 @@
         <f>('Full data'!C122)</f>
         <v>out of range options</v>
       </c>
-      <c r="D14" s="2" t="str">
-        <f>('Full data'!D122)</f>
-        <v>2015-05-15.10:39:04</v>
-      </c>
       <c r="E14" s="10" t="s">
         <v>136</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="2" t="str">
-        <f>('Full data'!H122)</f>
-        <v xml:space="preserve">Row: 1 Column: 1 Row: 2 Column: 3 Row: 4 Column: 5 </v>
-      </c>
       <c r="I14" s="2" t="str">
         <f>('Full data'!I122)</f>
         <v>Z</v>
       </c>
-      <c r="J14" s="2" t="str">
-        <f>('Full data'!J122)</f>
-        <v>[20,20](0,0)(19,19)(5,3,1,10)(5,4,13,1)(2,2,1,10)(10,10,5,5))</v>
-      </c>
-      <c r="K14" s="2" t="str">
-        <f>('Full data'!K122)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AE14" s="2" t="s">
         <v>25</v>
       </c>
@@ -10914,7 +10699,7 @@
       <c r="AG14" s="5"/>
       <c r="AI14" s="5"/>
     </row>
-    <row r="15" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>('Full data'!A132)</f>
         <v>Simulation</v>
@@ -10927,10 +10712,6 @@
         <f>('Full data'!C132)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="str">
-        <f>('Full data'!D132)</f>
-        <v>2015-05-15.10:39:43</v>
-      </c>
       <c r="E15" s="10" t="s">
         <v>137</v>
       </c>
@@ -10942,22 +10723,10 @@
         <f>('Full data'!G132)</f>
         <v>27</v>
       </c>
-      <c r="H15" s="2" t="str">
-        <f>('Full data'!H132)</f>
-        <v xml:space="preserve">Row: 7 Column: 5 Row: 14 Column: 6 Row: 20 Column: 13 </v>
-      </c>
       <c r="I15" s="2" t="str">
         <f>('Full data'!I132)</f>
         <v>Z</v>
       </c>
-      <c r="J15" s="2" t="str">
-        <f>('Full data'!J132)</f>
-        <v>[20,20](0,0)(19,19)(5,3,1,10)(5,4,13,1)(2,2,1,10)(10,10,5,5))</v>
-      </c>
-      <c r="K15" s="2" t="str">
-        <f>('Full data'!K132)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF15" s="2" t="s">
         <v>137</v>
       </c>
@@ -10975,7 +10744,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>('Full data'!A142)</f>
         <v>Simulation</v>
@@ -10988,10 +10757,6 @@
         <f>('Full data'!C142)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="str">
-        <f>('Full data'!D142)</f>
-        <v>2015-05-15.10:40:06</v>
-      </c>
       <c r="E16" s="10" t="s">
         <v>138</v>
       </c>
@@ -11003,22 +10768,10 @@
         <f>('Full data'!G142)</f>
         <v>52</v>
       </c>
-      <c r="H16" s="2" t="str">
-        <f>('Full data'!H142)</f>
-        <v xml:space="preserve">Row: 2 Column: 2 Row: 5 Column: 5 Row: 14 Column: 8 </v>
-      </c>
       <c r="I16" s="2" t="str">
         <f>('Full data'!I142)</f>
         <v>Z</v>
       </c>
-      <c r="J16" s="2" t="str">
-        <f>('Full data'!J142)</f>
-        <v>[20,20](0,0)(19,19)(5,3,1,10)(5,4,13,1)(2,2,1,10)(10,10,5,5))</v>
-      </c>
-      <c r="K16" s="2" t="str">
-        <f>('Full data'!K142)</f>
-        <v>3(2,3,5,9,15,20))</v>
-      </c>
       <c r="AF16" s="2" t="s">
         <v>138</v>
       </c>
@@ -11036,7 +10789,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f>('Full data'!A152)</f>
         <v>Simulation</v>
@@ -11049,10 +10802,6 @@
         <f>('Full data'!C152)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="2" t="str">
-        <f>('Full data'!D152)</f>
-        <v>2015-05-15.10:40:28</v>
-      </c>
       <c r="E17" s="10" t="s">
         <v>139</v>
       </c>
@@ -11064,21 +10813,9 @@
         <f>('Full data'!G152)</f>
         <v>44</v>
       </c>
-      <c r="H17" s="2" t="str">
-        <f>('Full data'!H152)</f>
-        <v xml:space="preserve">Row: 9 Column: 5 Row: 13 Column: 7 Row: 20 Column: 13 </v>
-      </c>
       <c r="I17" s="2" t="str">
         <f>('Full data'!I152)</f>
         <v>Z</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f>('Full data'!J152)</f>
-        <v>[20,20](0,0)(19,19)(5,3,1,10)(5,4,13,1)(2,2,1,10)(10,10,5,5))</v>
-      </c>
-      <c r="K17" s="2" t="str">
-        <f>('Full data'!K152)</f>
-        <v>3(2,3,5,9,15,20))</v>
       </c>
       <c r="AF17" s="2" t="s">
         <v>139</v>

</xml_diff>